<commit_message>
Update riaps package version number for release 1.1.23
</commit_message>
<xml_diff>
--- a/RIAPS-PackageLists.xlsx
+++ b/RIAPS-PackageLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metelko/Documents/RIAPS/RIAPS_GITHUB/riaps-integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6482C611-EBEA-B142-84DB-6070869B5642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA38559-7505-0B45-9E12-1889FEA58E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="4720" windowWidth="38340" windowHeight="18880" xr2:uid="{7E603EFB-FC55-574C-8736-016C25875C1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29360" windowHeight="18880" xr2:uid="{7E603EFB-FC55-574C-8736-016C25875C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="RIAPS Platform Specific" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{24BC86E9-6E42-C043-8518-DCC589AFEA71}" name="bbb-pkg" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/metelko/Downloads/RIAPS/release-1.1.22/info-for-manifest/bbb-pkg.txt" delimited="0">
+    <textPr sourceFile="/Users/metelko/Downloads/RIAPS/release-1.1.22/info-for-manifest/bbb-pkg.txt" delimited="0">
       <textFields count="5">
         <textField type="text"/>
         <textField type="text" position="4"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17769" uniqueCount="6139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17769" uniqueCount="6140">
   <si>
     <t>Python Package</t>
   </si>
@@ -18249,9 +18249,6 @@
     <t>3.0.2</t>
   </si>
   <si>
-    <t>Release Version: 1.1.22</t>
-  </si>
-  <si>
     <t>XUbuntu 20.04</t>
   </si>
   <si>
@@ -18526,6 +18523,12 @@
   </si>
   <si>
     <t>rtl8821cu-modules-5.10.168-ti-rt-r71</t>
+  </si>
+  <si>
+    <t>1.1.23</t>
+  </si>
+  <si>
+    <t>Release Version: 1.1.23</t>
   </si>
 </sst>
 </file>
@@ -19183,7 +19186,7 @@
   <dimension ref="B1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19199,18 +19202,18 @@
   <sheetData>
     <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="50" t="s">
-        <v>6048</v>
+        <v>6047</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>4483</v>
+        <v>6138</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="50" t="s">
-        <v>6049</v>
+        <v>6048</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>6047</v>
+        <v>6046</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -19222,7 +19225,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>6050</v>
+        <v>6049</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>5991</v>
@@ -19261,7 +19264,7 @@
         <v>5994</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>6052</v>
+        <v>6051</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="17" x14ac:dyDescent="0.2">
@@ -19337,7 +19340,7 @@
         <v>6000</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>6059</v>
+        <v>6058</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -19387,7 +19390,7 @@
         <v>6005</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>6051</v>
+        <v>6050</v>
       </c>
     </row>
     <row r="18" spans="4:7" ht="17" x14ac:dyDescent="0.2">
@@ -19413,7 +19416,7 @@
         <v>6008</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>6053</v>
+        <v>6052</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19451,7 +19454,7 @@
         <v>6011</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>6054</v>
+        <v>6053</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="17" x14ac:dyDescent="0.2">
@@ -19465,7 +19468,7 @@
         <v>6012</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>6056</v>
+        <v>6055</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -19491,7 +19494,7 @@
         <v>6014</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>6055</v>
+        <v>6054</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -19550,7 +19553,7 @@
         <v>4230</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>6057</v>
+        <v>6056</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>6019</v>
@@ -19579,7 +19582,7 @@
         <v>6020</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>6054</v>
+        <v>6053</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -19593,7 +19596,7 @@
         <v>6021</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>6058</v>
+        <v>6057</v>
       </c>
     </row>
     <row r="34" spans="3:7" ht="17" x14ac:dyDescent="0.2">
@@ -19657,7 +19660,7 @@
         <v>6027</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>6059</v>
+        <v>6058</v>
       </c>
     </row>
     <row r="39" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -19914,8 +19917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE93030E-850E-F044-9EBE-AA18D0F9328F}">
   <dimension ref="B1:J2117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A1879" workbookViewId="0">
+      <selection activeCell="D1908" sqref="D1908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19931,33 +19934,33 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>6046</v>
+        <v>6139</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>6060</v>
+        <v>6059</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>6063</v>
+        <v>6062</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
+        <v>6115</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6116</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6117</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
+        <v>6117</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6118</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6119</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>106</v>
@@ -19965,10 +19968,10 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
+        <v>6119</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6120</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6121</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>108</v>
@@ -19999,10 +20002,10 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
+        <v>6121</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>6122</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6123</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>115</v>
@@ -20011,7 +20014,7 @@
         <v>116</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>6124</v>
+        <v>6123</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>5786</v>
@@ -20258,7 +20261,7 @@
         <v>149</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6064</v>
+        <v>6063</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>119</v>
@@ -20350,7 +20353,7 @@
         <v>159</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>6065</v>
+        <v>6064</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>132</v>
@@ -20373,7 +20376,7 @@
         <v>162</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>6065</v>
+        <v>6064</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>132</v>
@@ -21615,7 +21618,7 @@
         <v>300</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>6066</v>
+        <v>6065</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>132</v>
@@ -22098,7 +22101,7 @@
         <v>355</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>119</v>
@@ -22121,7 +22124,7 @@
         <v>356</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>119</v>
@@ -22305,7 +22308,7 @@
         <v>373</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>119</v>
@@ -22328,7 +22331,7 @@
         <v>375</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>6069</v>
+        <v>6068</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>119</v>
@@ -22351,7 +22354,7 @@
         <v>377</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>119</v>
@@ -22374,7 +22377,7 @@
         <v>379</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>119</v>
@@ -22397,7 +22400,7 @@
         <v>381</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>132</v>
@@ -22420,7 +22423,7 @@
         <v>383</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>119</v>
@@ -22443,7 +22446,7 @@
         <v>385</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>119</v>
@@ -22466,7 +22469,7 @@
         <v>387</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>6069</v>
+        <v>6068</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>119</v>
@@ -22489,7 +22492,7 @@
         <v>389</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>6069</v>
+        <v>6068</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>119</v>
@@ -22512,7 +22515,7 @@
         <v>391</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>119</v>
@@ -22558,7 +22561,7 @@
         <v>396</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>119</v>
@@ -22581,7 +22584,7 @@
         <v>398</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>132</v>
@@ -23465,7 +23468,7 @@
         <v>523</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>6070</v>
+        <v>6069</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>119</v>
@@ -23482,7 +23485,7 @@
         <v>525</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>6070</v>
+        <v>6069</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>119</v>
@@ -24298,7 +24301,7 @@
         <v>656</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>6071</v>
+        <v>6070</v>
       </c>
       <c r="E216" s="2" t="s">
         <v>132</v>
@@ -25386,7 +25389,7 @@
         <v>811</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>6072</v>
+        <v>6071</v>
       </c>
       <c r="E280" s="2" t="s">
         <v>119</v>
@@ -25403,7 +25406,7 @@
         <v>813</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>6073</v>
+        <v>6072</v>
       </c>
       <c r="E281" s="2" t="s">
         <v>119</v>
@@ -25454,7 +25457,7 @@
         <v>818</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E284" s="2" t="s">
         <v>119</v>
@@ -25471,7 +25474,7 @@
         <v>820</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E285" s="2" t="s">
         <v>119</v>
@@ -25590,7 +25593,7 @@
         <v>832</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E292" s="2" t="s">
         <v>132</v>
@@ -25624,7 +25627,7 @@
         <v>835</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E294" s="2" t="s">
         <v>119</v>
@@ -25641,7 +25644,7 @@
         <v>837</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E295" s="2" t="s">
         <v>119</v>
@@ -25658,7 +25661,7 @@
         <v>838</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E296" s="2" t="s">
         <v>119</v>
@@ -25675,7 +25678,7 @@
         <v>840</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E297" s="2" t="s">
         <v>119</v>
@@ -25743,7 +25746,7 @@
         <v>844</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E301" s="2" t="s">
         <v>132</v>
@@ -25913,7 +25916,7 @@
         <v>868</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>6075</v>
+        <v>6074</v>
       </c>
       <c r="E311" s="2" t="s">
         <v>119</v>
@@ -25930,7 +25933,7 @@
         <v>870</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>6075</v>
+        <v>6074</v>
       </c>
       <c r="E312" s="2" t="s">
         <v>119</v>
@@ -26236,7 +26239,7 @@
         <v>917</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E330" s="2" t="s">
         <v>119</v>
@@ -26304,7 +26307,7 @@
         <v>928</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>6077</v>
+        <v>6076</v>
       </c>
       <c r="E334" s="2" t="s">
         <v>119</v>
@@ -26491,7 +26494,7 @@
         <v>960</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>6077</v>
+        <v>6076</v>
       </c>
       <c r="E345" s="2" t="s">
         <v>119</v>
@@ -26899,7 +26902,7 @@
         <v>1016</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>6078</v>
+        <v>6077</v>
       </c>
       <c r="E369" s="2" t="s">
         <v>119</v>
@@ -27069,7 +27072,7 @@
         <v>1037</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>6079</v>
+        <v>6078</v>
       </c>
       <c r="E379" s="2" t="s">
         <v>119</v>
@@ -27256,7 +27259,7 @@
         <v>1063</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E390" s="2" t="s">
         <v>119</v>
@@ -27273,7 +27276,7 @@
         <v>1065</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E391" s="2" t="s">
         <v>119</v>
@@ -27341,7 +27344,7 @@
         <v>1076</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E395" s="2" t="s">
         <v>119</v>
@@ -27358,7 +27361,7 @@
         <v>1078</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E396" s="2" t="s">
         <v>119</v>
@@ -27375,7 +27378,7 @@
         <v>1080</v>
       </c>
       <c r="D397" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E397" s="2" t="s">
         <v>119</v>
@@ -27409,7 +27412,7 @@
         <v>1084</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E399" s="2" t="s">
         <v>119</v>
@@ -27902,7 +27905,7 @@
         <v>1163</v>
       </c>
       <c r="D428" s="2" t="s">
-        <v>6080</v>
+        <v>6079</v>
       </c>
       <c r="E428" s="2" t="s">
         <v>119</v>
@@ -27919,7 +27922,7 @@
         <v>1165</v>
       </c>
       <c r="D429" s="2" t="s">
-        <v>6081</v>
+        <v>6080</v>
       </c>
       <c r="E429" s="2" t="s">
         <v>119</v>
@@ -28089,7 +28092,7 @@
         <v>1190</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>6082</v>
+        <v>6081</v>
       </c>
       <c r="E439" s="2" t="s">
         <v>119</v>
@@ -29109,7 +29112,7 @@
         <v>1335</v>
       </c>
       <c r="D499" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E499" s="2" t="s">
         <v>132</v>
@@ -29126,7 +29129,7 @@
         <v>1336</v>
       </c>
       <c r="D500" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E500" s="2" t="s">
         <v>132</v>
@@ -29483,7 +29486,7 @@
         <v>1384</v>
       </c>
       <c r="D521" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E521" s="2" t="s">
         <v>132</v>
@@ -29500,7 +29503,7 @@
         <v>1385</v>
       </c>
       <c r="D522" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E522" s="2" t="s">
         <v>132</v>
@@ -31863,7 +31866,7 @@
         <v>1673</v>
       </c>
       <c r="D661" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E661" s="2" t="s">
         <v>119</v>
@@ -31880,7 +31883,7 @@
         <v>1675</v>
       </c>
       <c r="D662" s="2" t="s">
-        <v>6069</v>
+        <v>6068</v>
       </c>
       <c r="E662" s="2" t="s">
         <v>119</v>
@@ -31897,7 +31900,7 @@
         <v>1677</v>
       </c>
       <c r="D663" s="2" t="s">
-        <v>6068</v>
+        <v>6067</v>
       </c>
       <c r="E663" s="2" t="s">
         <v>119</v>
@@ -32577,7 +32580,7 @@
         <v>1768</v>
       </c>
       <c r="D703" s="2" t="s">
-        <v>6083</v>
+        <v>6082</v>
       </c>
       <c r="E703" s="2" t="s">
         <v>119</v>
@@ -32696,7 +32699,7 @@
         <v>1787</v>
       </c>
       <c r="D710" s="2" t="s">
-        <v>6083</v>
+        <v>6082</v>
       </c>
       <c r="E710" s="2" t="s">
         <v>119</v>
@@ -33206,7 +33209,7 @@
         <v>1856</v>
       </c>
       <c r="D740" s="2" t="s">
-        <v>6084</v>
+        <v>6083</v>
       </c>
       <c r="E740" s="2" t="s">
         <v>119</v>
@@ -33665,7 +33668,7 @@
         <v>1925</v>
       </c>
       <c r="D767" s="2" t="s">
-        <v>6069</v>
+        <v>6068</v>
       </c>
       <c r="E767" s="2" t="s">
         <v>119</v>
@@ -33767,7 +33770,7 @@
         <v>1940</v>
       </c>
       <c r="D773" s="2" t="s">
-        <v>6072</v>
+        <v>6071</v>
       </c>
       <c r="E773" s="2" t="s">
         <v>119</v>
@@ -33801,7 +33804,7 @@
         <v>1945</v>
       </c>
       <c r="D775" s="2" t="s">
-        <v>6072</v>
+        <v>6071</v>
       </c>
       <c r="E775" s="2" t="s">
         <v>119</v>
@@ -34022,7 +34025,7 @@
         <v>1972</v>
       </c>
       <c r="D788" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E788" s="2" t="s">
         <v>132</v>
@@ -34039,7 +34042,7 @@
         <v>1973</v>
       </c>
       <c r="D789" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E789" s="2" t="s">
         <v>132</v>
@@ -34107,7 +34110,7 @@
         <v>1978</v>
       </c>
       <c r="D793" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E793" s="2" t="s">
         <v>132</v>
@@ -34124,7 +34127,7 @@
         <v>1980</v>
       </c>
       <c r="D794" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E794" s="2" t="s">
         <v>132</v>
@@ -35161,7 +35164,7 @@
         <v>2104</v>
       </c>
       <c r="D855" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E855" s="2" t="s">
         <v>132</v>
@@ -35178,7 +35181,7 @@
         <v>2105</v>
       </c>
       <c r="D856" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E856" s="2" t="s">
         <v>132</v>
@@ -35263,7 +35266,7 @@
         <v>2113</v>
       </c>
       <c r="D861" s="2" t="s">
-        <v>6085</v>
+        <v>6084</v>
       </c>
       <c r="E861" s="2" t="s">
         <v>119</v>
@@ -35280,7 +35283,7 @@
         <v>2116</v>
       </c>
       <c r="D862" s="2" t="s">
-        <v>6085</v>
+        <v>6084</v>
       </c>
       <c r="E862" s="2" t="s">
         <v>119</v>
@@ -35552,7 +35555,7 @@
         <v>2146</v>
       </c>
       <c r="D878" s="2" t="s">
-        <v>6075</v>
+        <v>6074</v>
       </c>
       <c r="E878" s="2" t="s">
         <v>119</v>
@@ -35569,7 +35572,7 @@
         <v>2148</v>
       </c>
       <c r="D879" s="2" t="s">
-        <v>6075</v>
+        <v>6074</v>
       </c>
       <c r="E879" s="2" t="s">
         <v>132</v>
@@ -35807,7 +35810,7 @@
         <v>2173</v>
       </c>
       <c r="D893" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E893" s="2" t="s">
         <v>119</v>
@@ -35841,7 +35844,7 @@
         <v>2177</v>
       </c>
       <c r="D895" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E895" s="2" t="s">
         <v>119</v>
@@ -35858,7 +35861,7 @@
         <v>2179</v>
       </c>
       <c r="D896" s="2" t="s">
-        <v>6076</v>
+        <v>6075</v>
       </c>
       <c r="E896" s="2" t="s">
         <v>119</v>
@@ -37405,7 +37408,7 @@
         <v>2392</v>
       </c>
       <c r="D987" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E987" s="2" t="s">
         <v>132</v>
@@ -37473,7 +37476,7 @@
         <v>2402</v>
       </c>
       <c r="D991" s="2" t="s">
-        <v>6077</v>
+        <v>6076</v>
       </c>
       <c r="E991" s="2" t="s">
         <v>119</v>
@@ -37762,7 +37765,7 @@
         <v>2440</v>
       </c>
       <c r="D1008" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1008" s="2" t="s">
         <v>132</v>
@@ -37779,7 +37782,7 @@
         <v>2442</v>
       </c>
       <c r="D1009" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1009" s="2" t="s">
         <v>132</v>
@@ -38119,7 +38122,7 @@
         <v>2475</v>
       </c>
       <c r="D1029" s="2" t="s">
-        <v>6087</v>
+        <v>6086</v>
       </c>
       <c r="E1029" s="2" t="s">
         <v>119</v>
@@ -38782,7 +38785,7 @@
         <v>2553</v>
       </c>
       <c r="D1068" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1068" s="2" t="s">
         <v>132</v>
@@ -39700,7 +39703,7 @@
         <v>2681</v>
       </c>
       <c r="D1122" s="2" t="s">
-        <v>6088</v>
+        <v>6087</v>
       </c>
       <c r="E1122" s="2" t="s">
         <v>119</v>
@@ -41791,7 +41794,7 @@
         <v>2948</v>
       </c>
       <c r="D1245" s="2" t="s">
-        <v>6089</v>
+        <v>6088</v>
       </c>
       <c r="E1245" s="2" t="s">
         <v>119</v>
@@ -41808,7 +41811,7 @@
         <v>2950</v>
       </c>
       <c r="D1246" s="2" t="s">
-        <v>6089</v>
+        <v>6088</v>
       </c>
       <c r="E1246" s="2" t="s">
         <v>119</v>
@@ -41825,7 +41828,7 @@
         <v>2952</v>
       </c>
       <c r="D1247" s="2" t="s">
-        <v>6089</v>
+        <v>6088</v>
       </c>
       <c r="E1247" s="2" t="s">
         <v>119</v>
@@ -42539,7 +42542,7 @@
         <v>3040</v>
       </c>
       <c r="D1289" s="2" t="s">
-        <v>6090</v>
+        <v>6089</v>
       </c>
       <c r="E1289" s="2" t="s">
         <v>119</v>
@@ -42675,7 +42678,7 @@
         <v>3054</v>
       </c>
       <c r="D1297" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1297" s="2" t="s">
         <v>119</v>
@@ -42692,7 +42695,7 @@
         <v>3056</v>
       </c>
       <c r="D1298" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1298" s="2" t="s">
         <v>119</v>
@@ -42709,7 +42712,7 @@
         <v>3058</v>
       </c>
       <c r="D1299" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1299" s="2" t="s">
         <v>132</v>
@@ -42726,7 +42729,7 @@
         <v>3060</v>
       </c>
       <c r="D1300" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1300" s="2" t="s">
         <v>119</v>
@@ -42743,7 +42746,7 @@
         <v>3062</v>
       </c>
       <c r="D1301" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1301" s="2" t="s">
         <v>119</v>
@@ -42760,7 +42763,7 @@
         <v>3064</v>
       </c>
       <c r="D1302" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1302" s="2" t="s">
         <v>119</v>
@@ -42777,7 +42780,7 @@
         <v>3066</v>
       </c>
       <c r="D1303" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1303" s="2" t="s">
         <v>119</v>
@@ -42794,7 +42797,7 @@
         <v>3068</v>
       </c>
       <c r="D1304" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1304" s="2" t="s">
         <v>132</v>
@@ -42811,7 +42814,7 @@
         <v>3070</v>
       </c>
       <c r="D1305" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1305" s="2" t="s">
         <v>132</v>
@@ -42828,7 +42831,7 @@
         <v>3072</v>
       </c>
       <c r="D1306" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1306" s="2" t="s">
         <v>119</v>
@@ -42845,7 +42848,7 @@
         <v>3074</v>
       </c>
       <c r="D1307" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1307" s="2" t="s">
         <v>119</v>
@@ -42862,7 +42865,7 @@
         <v>3076</v>
       </c>
       <c r="D1308" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1308" s="2" t="s">
         <v>132</v>
@@ -42879,7 +42882,7 @@
         <v>3078</v>
       </c>
       <c r="D1309" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1309" s="2" t="s">
         <v>132</v>
@@ -42896,7 +42899,7 @@
         <v>3080</v>
       </c>
       <c r="D1310" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1310" s="2" t="s">
         <v>132</v>
@@ -42913,7 +42916,7 @@
         <v>3082</v>
       </c>
       <c r="D1311" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1311" s="2" t="s">
         <v>119</v>
@@ -42981,7 +42984,7 @@
         <v>3093</v>
       </c>
       <c r="D1315" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1315" s="2" t="s">
         <v>132</v>
@@ -43049,7 +43052,7 @@
         <v>3099</v>
       </c>
       <c r="D1319" s="2" t="s">
-        <v>6091</v>
+        <v>6090</v>
       </c>
       <c r="E1319" s="2" t="s">
         <v>119</v>
@@ -43066,7 +43069,7 @@
         <v>3101</v>
       </c>
       <c r="D1320" s="2" t="s">
-        <v>6091</v>
+        <v>6090</v>
       </c>
       <c r="E1320" s="2" t="s">
         <v>119</v>
@@ -43712,7 +43715,7 @@
         <v>3187</v>
       </c>
       <c r="D1358" s="2" t="s">
-        <v>6092</v>
+        <v>6091</v>
       </c>
       <c r="E1358" s="2" t="s">
         <v>119</v>
@@ -43814,7 +43817,7 @@
         <v>3202</v>
       </c>
       <c r="D1364" s="2" t="s">
-        <v>6093</v>
+        <v>6092</v>
       </c>
       <c r="E1364" s="2" t="s">
         <v>132</v>
@@ -43831,7 +43834,7 @@
         <v>3204</v>
       </c>
       <c r="D1365" s="2" t="s">
-        <v>6093</v>
+        <v>6092</v>
       </c>
       <c r="E1365" s="2" t="s">
         <v>119</v>
@@ -44494,7 +44497,7 @@
         <v>3281</v>
       </c>
       <c r="D1404" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E1404" s="2" t="s">
         <v>132</v>
@@ -44511,7 +44514,7 @@
         <v>3283</v>
       </c>
       <c r="D1405" s="2" t="s">
-        <v>6067</v>
+        <v>6066</v>
       </c>
       <c r="E1405" s="2" t="s">
         <v>132</v>
@@ -44579,7 +44582,7 @@
         <v>3289</v>
       </c>
       <c r="D1409" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1409" s="2" t="s">
         <v>132</v>
@@ -44596,7 +44599,7 @@
         <v>3291</v>
       </c>
       <c r="D1410" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1410" s="2" t="s">
         <v>132</v>
@@ -44681,7 +44684,7 @@
         <v>3302</v>
       </c>
       <c r="D1415" s="2" t="s">
-        <v>6087</v>
+        <v>6086</v>
       </c>
       <c r="E1415" s="2" t="s">
         <v>119</v>
@@ -45157,7 +45160,7 @@
         <v>3366</v>
       </c>
       <c r="D1443" s="2" t="s">
-        <v>6094</v>
+        <v>6093</v>
       </c>
       <c r="E1443" s="2" t="s">
         <v>119</v>
@@ -45378,7 +45381,7 @@
         <v>3393</v>
       </c>
       <c r="D1456" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1456" s="2" t="s">
         <v>132</v>
@@ -45514,7 +45517,7 @@
         <v>3410</v>
       </c>
       <c r="D1464" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1464" s="2" t="s">
         <v>132</v>
@@ -45531,7 +45534,7 @@
         <v>3411</v>
       </c>
       <c r="D1465" s="2" t="s">
-        <v>6074</v>
+        <v>6073</v>
       </c>
       <c r="E1465" s="2" t="s">
         <v>132</v>
@@ -45752,7 +45755,7 @@
         <v>3440</v>
       </c>
       <c r="D1478" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1478" s="2" t="s">
         <v>119</v>
@@ -45769,7 +45772,7 @@
         <v>3442</v>
       </c>
       <c r="D1479" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1479" s="2" t="s">
         <v>119</v>
@@ -45786,7 +45789,7 @@
         <v>3444</v>
       </c>
       <c r="D1480" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1480" s="2" t="s">
         <v>119</v>
@@ -45803,7 +45806,7 @@
         <v>3446</v>
       </c>
       <c r="D1481" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1481" s="2" t="s">
         <v>119</v>
@@ -45820,7 +45823,7 @@
         <v>3448</v>
       </c>
       <c r="D1482" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1482" s="2" t="s">
         <v>119</v>
@@ -45837,7 +45840,7 @@
         <v>3450</v>
       </c>
       <c r="D1483" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1483" s="2" t="s">
         <v>132</v>
@@ -46517,7 +46520,7 @@
         <v>3550</v>
       </c>
       <c r="D1523" s="2" t="s">
-        <v>6092</v>
+        <v>6091</v>
       </c>
       <c r="E1523" s="2" t="s">
         <v>119</v>
@@ -46534,7 +46537,7 @@
         <v>3552</v>
       </c>
       <c r="D1524" s="2" t="s">
-        <v>6077</v>
+        <v>6076</v>
       </c>
       <c r="E1524" s="2" t="s">
         <v>119</v>
@@ -46551,7 +46554,7 @@
         <v>3554</v>
       </c>
       <c r="D1525" s="2" t="s">
-        <v>6095</v>
+        <v>6094</v>
       </c>
       <c r="E1525" s="2" t="s">
         <v>119</v>
@@ -46568,7 +46571,7 @@
         <v>3556</v>
       </c>
       <c r="D1526" s="2" t="s">
-        <v>6095</v>
+        <v>6094</v>
       </c>
       <c r="E1526" s="2" t="s">
         <v>119</v>
@@ -46585,7 +46588,7 @@
         <v>3557</v>
       </c>
       <c r="D1527" s="2" t="s">
-        <v>6095</v>
+        <v>6094</v>
       </c>
       <c r="E1527" s="2" t="s">
         <v>119</v>
@@ -48557,7 +48560,7 @@
         <v>3855</v>
       </c>
       <c r="D1643" s="2" t="s">
-        <v>6096</v>
+        <v>6095</v>
       </c>
       <c r="E1643" s="2" t="s">
         <v>119</v>
@@ -48588,10 +48591,10 @@
         <v>117</v>
       </c>
       <c r="C1645" s="2" t="s">
+        <v>6096</v>
+      </c>
+      <c r="D1645" s="2" t="s">
         <v>6097</v>
-      </c>
-      <c r="D1645" s="2" t="s">
-        <v>6098</v>
       </c>
       <c r="E1645" s="2" t="s">
         <v>119</v>
@@ -48608,7 +48611,7 @@
         <v>3861</v>
       </c>
       <c r="D1646" s="2" t="s">
-        <v>6096</v>
+        <v>6095</v>
       </c>
       <c r="E1646" s="2" t="s">
         <v>119</v>
@@ -48639,10 +48642,10 @@
         <v>117</v>
       </c>
       <c r="C1648" s="2" t="s">
-        <v>6099</v>
+        <v>6098</v>
       </c>
       <c r="D1648" s="2" t="s">
-        <v>6098</v>
+        <v>6097</v>
       </c>
       <c r="E1648" s="2" t="s">
         <v>132</v>
@@ -48690,10 +48693,10 @@
         <v>117</v>
       </c>
       <c r="C1651" s="2" t="s">
-        <v>6100</v>
+        <v>6099</v>
       </c>
       <c r="D1651" s="2" t="s">
-        <v>6098</v>
+        <v>6097</v>
       </c>
       <c r="E1651" s="2" t="s">
         <v>119</v>
@@ -48710,7 +48713,7 @@
         <v>3868</v>
       </c>
       <c r="D1652" s="2" t="s">
-        <v>6096</v>
+        <v>6095</v>
       </c>
       <c r="E1652" s="2" t="s">
         <v>119</v>
@@ -48727,7 +48730,7 @@
         <v>3870</v>
       </c>
       <c r="D1653" s="2" t="s">
-        <v>6101</v>
+        <v>6100</v>
       </c>
       <c r="E1653" s="2" t="s">
         <v>119</v>
@@ -48744,7 +48747,7 @@
         <v>3872</v>
       </c>
       <c r="D1654" s="2" t="s">
-        <v>6101</v>
+        <v>6100</v>
       </c>
       <c r="E1654" s="2" t="s">
         <v>333</v>
@@ -48761,7 +48764,7 @@
         <v>3873</v>
       </c>
       <c r="D1655" s="2" t="s">
-        <v>6101</v>
+        <v>6100</v>
       </c>
       <c r="E1655" s="2" t="s">
         <v>335</v>
@@ -48843,10 +48846,10 @@
         <v>117</v>
       </c>
       <c r="C1660" s="2" t="s">
-        <v>6102</v>
+        <v>6101</v>
       </c>
       <c r="D1660" s="2" t="s">
-        <v>6098</v>
+        <v>6097</v>
       </c>
       <c r="E1660" s="2" t="s">
         <v>119</v>
@@ -48894,10 +48897,10 @@
         <v>117</v>
       </c>
       <c r="C1663" s="2" t="s">
-        <v>6103</v>
+        <v>6102</v>
       </c>
       <c r="D1663" s="2" t="s">
-        <v>6098</v>
+        <v>6097</v>
       </c>
       <c r="E1663" s="2" t="s">
         <v>119</v>
@@ -49557,16 +49560,16 @@
         <v>117</v>
       </c>
       <c r="C1702" s="2" t="s">
+        <v>6103</v>
+      </c>
+      <c r="D1702" s="2" t="s">
         <v>6104</v>
       </c>
-      <c r="D1702" s="2" t="s">
+      <c r="E1702" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1702" s="2" t="s">
         <v>6105</v>
-      </c>
-      <c r="E1702" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1702" s="2" t="s">
-        <v>6106</v>
       </c>
     </row>
     <row r="1703" spans="2:6" x14ac:dyDescent="0.2">
@@ -49883,7 +49886,7 @@
         <v>4021</v>
       </c>
       <c r="D1721" s="2" t="s">
-        <v>6107</v>
+        <v>6106</v>
       </c>
       <c r="E1721" s="2" t="s">
         <v>119</v>
@@ -50019,7 +50022,7 @@
         <v>4041</v>
       </c>
       <c r="D1729" s="2" t="s">
-        <v>6108</v>
+        <v>6107</v>
       </c>
       <c r="E1729" s="2" t="s">
         <v>119</v>
@@ -50036,7 +50039,7 @@
         <v>4043</v>
       </c>
       <c r="D1730" s="2" t="s">
-        <v>6108</v>
+        <v>6107</v>
       </c>
       <c r="E1730" s="2" t="s">
         <v>119</v>
@@ -50053,7 +50056,7 @@
         <v>4045</v>
       </c>
       <c r="D1731" s="2" t="s">
-        <v>6109</v>
+        <v>6108</v>
       </c>
       <c r="E1731" s="2" t="s">
         <v>119</v>
@@ -50155,7 +50158,7 @@
         <v>4057</v>
       </c>
       <c r="D1737" s="2" t="s">
-        <v>6110</v>
+        <v>6109</v>
       </c>
       <c r="E1737" s="2" t="s">
         <v>119</v>
@@ -50172,7 +50175,7 @@
         <v>4059</v>
       </c>
       <c r="D1738" s="2" t="s">
-        <v>6110</v>
+        <v>6109</v>
       </c>
       <c r="E1738" s="2" t="s">
         <v>132</v>
@@ -50189,7 +50192,7 @@
         <v>4061</v>
       </c>
       <c r="D1739" s="2" t="s">
-        <v>6110</v>
+        <v>6109</v>
       </c>
       <c r="E1739" s="2" t="s">
         <v>119</v>
@@ -50206,7 +50209,7 @@
         <v>4063</v>
       </c>
       <c r="D1740" s="2" t="s">
-        <v>6110</v>
+        <v>6109</v>
       </c>
       <c r="E1740" s="2" t="s">
         <v>119</v>
@@ -50835,7 +50838,7 @@
         <v>4152</v>
       </c>
       <c r="D1777" s="2" t="s">
-        <v>6089</v>
+        <v>6088</v>
       </c>
       <c r="E1777" s="2" t="s">
         <v>119</v>
@@ -51498,7 +51501,7 @@
         <v>4249</v>
       </c>
       <c r="D1816" s="2" t="s">
-        <v>6065</v>
+        <v>6064</v>
       </c>
       <c r="E1816" s="2" t="s">
         <v>132</v>
@@ -51821,7 +51824,7 @@
         <v>4300</v>
       </c>
       <c r="D1835" s="2" t="s">
-        <v>6111</v>
+        <v>6110</v>
       </c>
       <c r="E1835" s="2" t="s">
         <v>132</v>
@@ -52331,7 +52334,7 @@
         <v>4380</v>
       </c>
       <c r="D1865" s="2" t="s">
-        <v>6110</v>
+        <v>6109</v>
       </c>
       <c r="E1865" s="2" t="s">
         <v>132</v>
@@ -52416,7 +52419,7 @@
         <v>4391</v>
       </c>
       <c r="D1870" s="2" t="s">
-        <v>6065</v>
+        <v>6064</v>
       </c>
       <c r="E1870" s="2" t="s">
         <v>132</v>
@@ -52518,7 +52521,7 @@
         <v>4406</v>
       </c>
       <c r="D1876" s="2" t="s">
-        <v>6112</v>
+        <v>6111</v>
       </c>
       <c r="E1876" s="2" t="s">
         <v>119</v>
@@ -52535,7 +52538,7 @@
         <v>4408</v>
       </c>
       <c r="D1877" s="2" t="s">
-        <v>6112</v>
+        <v>6111</v>
       </c>
       <c r="E1877" s="2" t="s">
         <v>132</v>
@@ -52552,7 +52555,7 @@
         <v>4410</v>
       </c>
       <c r="D1878" s="2" t="s">
-        <v>6112</v>
+        <v>6111</v>
       </c>
       <c r="E1878" s="2" t="s">
         <v>119</v>
@@ -52671,7 +52674,7 @@
         <v>4428</v>
       </c>
       <c r="D1885" s="2" t="s">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="E1885" s="2" t="s">
         <v>132</v>
@@ -52756,7 +52759,7 @@
         <v>4440</v>
       </c>
       <c r="D1890" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1890" s="2" t="s">
         <v>119</v>
@@ -53045,7 +53048,7 @@
         <v>4482</v>
       </c>
       <c r="D1907" s="2" t="s">
-        <v>4483</v>
+        <v>6138</v>
       </c>
       <c r="E1907" s="2" t="s">
         <v>132</v>
@@ -53062,7 +53065,7 @@
         <v>4485</v>
       </c>
       <c r="D1908" s="2" t="s">
-        <v>4483</v>
+        <v>6138</v>
       </c>
       <c r="E1908" s="2" t="s">
         <v>119</v>
@@ -53164,7 +53167,7 @@
         <v>4501</v>
       </c>
       <c r="D1914" s="2" t="s">
-        <v>6092</v>
+        <v>6091</v>
       </c>
       <c r="E1914" s="2" t="s">
         <v>119</v>
@@ -53402,7 +53405,7 @@
         <v>4541</v>
       </c>
       <c r="D1928" s="2" t="s">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="E1928" s="2" t="s">
         <v>132</v>
@@ -53419,7 +53422,7 @@
         <v>4543</v>
       </c>
       <c r="D1929" s="2" t="s">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="E1929" s="2" t="s">
         <v>132</v>
@@ -53929,7 +53932,7 @@
         <v>4620</v>
       </c>
       <c r="D1959" s="2" t="s">
-        <v>6114</v>
+        <v>6113</v>
       </c>
       <c r="E1959" s="2" t="s">
         <v>119</v>
@@ -53946,7 +53949,7 @@
         <v>4622</v>
       </c>
       <c r="D1960" s="2" t="s">
-        <v>6114</v>
+        <v>6113</v>
       </c>
       <c r="E1960" s="2" t="s">
         <v>119</v>
@@ -53963,7 +53966,7 @@
         <v>4624</v>
       </c>
       <c r="D1961" s="2" t="s">
-        <v>6114</v>
+        <v>6113</v>
       </c>
       <c r="E1961" s="2" t="s">
         <v>132</v>
@@ -54371,7 +54374,7 @@
         <v>4682</v>
       </c>
       <c r="D1985" s="2" t="s">
-        <v>6115</v>
+        <v>6114</v>
       </c>
       <c r="E1985" s="2" t="s">
         <v>132</v>
@@ -54405,7 +54408,7 @@
         <v>4688</v>
       </c>
       <c r="D1987" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1987" s="2" t="s">
         <v>119</v>
@@ -54541,7 +54544,7 @@
         <v>4706</v>
       </c>
       <c r="D1995" s="2" t="s">
-        <v>6086</v>
+        <v>6085</v>
       </c>
       <c r="E1995" s="2" t="s">
         <v>119</v>
@@ -56633,8 +56636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFE8052-1344-C141-9A09-091A05FE980D}">
   <dimension ref="B1:I729"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A647" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -56650,17 +56653,17 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>6046</v>
+        <v>6139</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>6061</v>
+        <v>6060</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>6062</v>
+        <v>6061</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -69625,7 +69628,7 @@
   <dimension ref="B1:I569"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -69641,33 +69644,33 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>6046</v>
+        <v>6139</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>6060</v>
+        <v>6059</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>6125</v>
+        <v>6124</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
+        <v>6115</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6116</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6117</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
+        <v>6117</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6118</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6119</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>106</v>
@@ -69675,10 +69678,10 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
+        <v>6119</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6120</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6121</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>108</v>
@@ -69709,13 +69712,13 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
+        <v>6121</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>6122</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>6123</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>6126</v>
+        <v>6125</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>116</v>
@@ -70379,16 +70382,16 @@
         <v>117</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>6126</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>6127</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>6128</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>335</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>6129</v>
+        <v>6128</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>39</v>
@@ -70405,7 +70408,7 @@
         <v>5055</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>6128</v>
+        <v>6127</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>335</v>
@@ -73878,7 +73881,7 @@
         <v>5179</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>6083</v>
+        <v>6082</v>
       </c>
       <c r="E232" s="2" t="s">
         <v>335</v>
@@ -76119,7 +76122,7 @@
         <v>117</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>6130</v>
+        <v>6129</v>
       </c>
       <c r="D364" s="2" t="s">
         <v>5274</v>
@@ -77224,7 +77227,7 @@
         <v>117</v>
       </c>
       <c r="C429" s="2" t="s">
-        <v>6131</v>
+        <v>6130</v>
       </c>
       <c r="D429" s="2" t="s">
         <v>5274</v>
@@ -77233,7 +77236,7 @@
         <v>335</v>
       </c>
       <c r="F429" s="2" t="s">
-        <v>6132</v>
+        <v>6131</v>
       </c>
     </row>
     <row r="430" spans="2:6" x14ac:dyDescent="0.2">
@@ -77244,7 +77247,7 @@
         <v>3873</v>
       </c>
       <c r="D430" s="2" t="s">
-        <v>6101</v>
+        <v>6100</v>
       </c>
       <c r="E430" s="2" t="s">
         <v>335</v>
@@ -78536,7 +78539,7 @@
         <v>4428</v>
       </c>
       <c r="D506" s="2" t="s">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="E506" s="2" t="s">
         <v>132</v>
@@ -78652,7 +78655,7 @@
         <v>117</v>
       </c>
       <c r="C513" s="2" t="s">
-        <v>6133</v>
+        <v>6132</v>
       </c>
       <c r="D513" s="2" t="s">
         <v>5274</v>
@@ -78729,7 +78732,7 @@
         <v>132</v>
       </c>
       <c r="F517" s="2" t="s">
-        <v>6134</v>
+        <v>6133</v>
       </c>
     </row>
     <row r="518" spans="2:6" x14ac:dyDescent="0.2">
@@ -78737,7 +78740,7 @@
         <v>117</v>
       </c>
       <c r="C518" s="2" t="s">
-        <v>6135</v>
+        <v>6134</v>
       </c>
       <c r="D518" s="2" t="s">
         <v>4483</v>
@@ -78805,7 +78808,7 @@
         <v>117</v>
       </c>
       <c r="C522" s="2" t="s">
-        <v>6136</v>
+        <v>6135</v>
       </c>
       <c r="D522" s="2" t="s">
         <v>5274</v>
@@ -78822,7 +78825,7 @@
         <v>117</v>
       </c>
       <c r="C523" s="2" t="s">
-        <v>6137</v>
+        <v>6136</v>
       </c>
       <c r="D523" s="2" t="s">
         <v>5274</v>
@@ -78839,7 +78842,7 @@
         <v>117</v>
       </c>
       <c r="C524" s="2" t="s">
-        <v>6138</v>
+        <v>6137</v>
       </c>
       <c r="D524" s="2" t="s">
         <v>5274</v>
@@ -78910,7 +78913,7 @@
         <v>4541</v>
       </c>
       <c r="D528" s="2" t="s">
-        <v>6113</v>
+        <v>6112</v>
       </c>
       <c r="E528" s="2" t="s">
         <v>132</v>

</xml_diff>